<commit_message>
evaluaciones heuristicas, e impacto iniciales
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -4,20 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" firstSheet="1" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Usabilidad" sheetId="1" r:id="rId1"/>
     <sheet name="Usuarios" sheetId="3" r:id="rId2"/>
     <sheet name="Heurística" sheetId="4" r:id="rId3"/>
     <sheet name="UE y H" sheetId="2" r:id="rId4"/>
+    <sheet name="Impacto S1" sheetId="5" r:id="rId5"/>
+    <sheet name="Impacto S7" sheetId="8" r:id="rId6"/>
+    <sheet name="Impacto S8" sheetId="6" r:id="rId7"/>
+    <sheet name="Impacto S9" sheetId="9" r:id="rId8"/>
+    <sheet name="Impacto S10" sheetId="7" r:id="rId9"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="113">
   <si>
     <t>Usabilidad</t>
   </si>
@@ -284,6 +289,78 @@
   </si>
   <si>
     <t>H2</t>
+  </si>
+  <si>
+    <t>Feedback cuando no hay obstáculso es insuficiente. Todo lo demás ok, muy entretenido y hay que conectrarse para responder ("acertijos") aunque no sean tan difíciles. Muy creativa la idea.</t>
+  </si>
+  <si>
+    <t>Las preguntas pueden cambiarse, pero como está es çoptimo para preguntas de geometría espacial.</t>
+  </si>
+  <si>
+    <t>Nicolás Delgado Vega</t>
+  </si>
+  <si>
+    <t>Américo Jerez Garcés</t>
+  </si>
+  <si>
+    <t>El tema tratado en el juego es matemáticas (orientación espacial y rotación/traslación), no toma cuestiones éticas o valóricas. La historia (en la demo) es simple y lineal, sin mucho como par encariñarse con los personajes (en este caso aprendiz y maestro). Gracias al juego me di cuenta que todavía me confundo con izquierda y dereacha.</t>
+  </si>
+  <si>
+    <t>Actualmente el juego es más una forma lúdica de verificar si los contenidos abordados son bien manejados o no por el jugador y no tanto para aprenderlos.</t>
+  </si>
+  <si>
+    <t>7º</t>
+  </si>
+  <si>
+    <t>Ceguera</t>
+  </si>
+  <si>
+    <t>Congenita</t>
+  </si>
+  <si>
+    <t>E Inicial</t>
+  </si>
+  <si>
+    <t>E Final</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>a)</t>
+  </si>
+  <si>
+    <t>Tickets Inicial</t>
+  </si>
+  <si>
+    <t>Tickets Final</t>
+  </si>
+  <si>
+    <t>Subtotal</t>
+  </si>
+  <si>
+    <t>b)</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>Pregunta</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Baja visión</t>
+  </si>
+  <si>
+    <t>15-17/11/2016</t>
   </si>
 </sst>
 </file>
@@ -319,13 +396,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,8 +700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -739,7 +817,9 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1906,15 +1986,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AY3"/>
+  <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1"/>
+    <sheetView topLeftCell="AK1" workbookViewId="0">
+      <selection activeCell="AZ4" sqref="AZ4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51">
+    <row r="1" spans="1:52">
       <c r="B1">
         <v>1</v>
       </c>
@@ -2065,8 +2145,11 @@
       <c r="AY1">
         <v>50</v>
       </c>
-    </row>
-    <row r="2" spans="1:51">
+      <c r="AZ1">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:52">
       <c r="A2" t="s">
         <v>87</v>
       </c>
@@ -2217,10 +2300,169 @@
       <c r="AX2">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:51">
+      <c r="AY2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="3" spans="1:52">
       <c r="A3" t="s">
         <v>88</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="E3">
+        <v>5</v>
+      </c>
+      <c r="F3">
+        <v>4</v>
+      </c>
+      <c r="G3">
+        <v>5</v>
+      </c>
+      <c r="H3">
+        <v>5</v>
+      </c>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>5</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>3</v>
+      </c>
+      <c r="N3">
+        <v>5</v>
+      </c>
+      <c r="O3">
+        <v>5</v>
+      </c>
+      <c r="P3">
+        <v>5</v>
+      </c>
+      <c r="Q3">
+        <v>4</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>4</v>
+      </c>
+      <c r="T3">
+        <v>4</v>
+      </c>
+      <c r="U3">
+        <v>4</v>
+      </c>
+      <c r="V3">
+        <v>3</v>
+      </c>
+      <c r="W3">
+        <v>5</v>
+      </c>
+      <c r="X3">
+        <v>5</v>
+      </c>
+      <c r="Y3">
+        <v>4</v>
+      </c>
+      <c r="Z3">
+        <v>5</v>
+      </c>
+      <c r="AA3">
+        <v>3</v>
+      </c>
+      <c r="AB3">
+        <v>5</v>
+      </c>
+      <c r="AC3">
+        <v>5</v>
+      </c>
+      <c r="AD3">
+        <v>5</v>
+      </c>
+      <c r="AE3">
+        <v>5</v>
+      </c>
+      <c r="AF3">
+        <v>5</v>
+      </c>
+      <c r="AG3">
+        <v>4</v>
+      </c>
+      <c r="AH3">
+        <v>5</v>
+      </c>
+      <c r="AI3">
+        <v>5</v>
+      </c>
+      <c r="AJ3">
+        <v>4</v>
+      </c>
+      <c r="AK3">
+        <v>5</v>
+      </c>
+      <c r="AL3">
+        <v>5</v>
+      </c>
+      <c r="AM3">
+        <v>5</v>
+      </c>
+      <c r="AN3">
+        <v>5</v>
+      </c>
+      <c r="AO3">
+        <v>5</v>
+      </c>
+      <c r="AP3">
+        <v>5</v>
+      </c>
+      <c r="AQ3">
+        <v>5</v>
+      </c>
+      <c r="AR3">
+        <v>5</v>
+      </c>
+      <c r="AS3">
+        <v>1</v>
+      </c>
+      <c r="AT3">
+        <v>3</v>
+      </c>
+      <c r="AU3">
+        <v>1</v>
+      </c>
+      <c r="AV3">
+        <v>0</v>
+      </c>
+      <c r="AW3">
+        <v>5</v>
+      </c>
+      <c r="AX3">
+        <v>5</v>
+      </c>
+      <c r="AY3" t="s">
+        <v>93</v>
+      </c>
+      <c r="AZ3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -2230,46 +2472,2630 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="10" spans="1:1">
+      <c r="B9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>88</v>
+      </c>
+      <c r="B10" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G49"/>
+  <sheetViews>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4">
+        <v>42689</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>2</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" t="s">
+        <v>106</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24">
+        <v>3</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="C26">
+        <v>5</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="C28">
+        <v>7</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="C29">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30" t="s">
+        <v>110</v>
+      </c>
+      <c r="D30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>108</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="F32">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="C34">
+        <v>3</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35">
+        <v>4</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36">
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <v>2</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38">
+        <v>7</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39">
+        <v>8</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="C40" t="s">
+        <v>110</v>
+      </c>
+      <c r="D40">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="C43">
+        <v>2</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="F43">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="C44">
+        <v>3</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45">
+        <v>4</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="C47">
+        <v>6</v>
+      </c>
+      <c r="D47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="C48">
+        <v>7</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49" t="s">
+        <v>110</v>
+      </c>
+      <c r="D49">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="F54" sqref="F54"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="4">
+        <v>42691</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="F38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6">
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="4">
+        <v>42689</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>4.5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="F35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="F40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="F44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6">
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F45" sqref="F45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>2</v>
+      </c>
+      <c r="F23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>2</v>
+      </c>
+      <c r="F27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:4">
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:4">
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G50"/>
+  <sheetViews>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4">
+        <v>42691</v>
+      </c>
+      <c r="C1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>2</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="C11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="B13" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="C17">
+        <v>5</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="C18">
+        <v>6</v>
+      </c>
+      <c r="D18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="C20" t="s">
+        <v>104</v>
+      </c>
+      <c r="D20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="C21" t="s">
+        <v>110</v>
+      </c>
+      <c r="D21">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" t="s">
+        <v>106</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="C25">
+        <v>3</v>
+      </c>
+      <c r="D25">
+        <v>2</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26">
+        <v>2</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="C27">
+        <v>5</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="C29">
+        <v>7</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="C30">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="C31" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>1</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="C34">
+        <v>2</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="C35">
+        <v>3</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
+      <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>2</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>2</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="F39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="C41" t="s">
+        <v>110</v>
+      </c>
+      <c r="D41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43">
+        <v>2</v>
+      </c>
+      <c r="F43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="C44">
+        <v>2</v>
+      </c>
+      <c r="D44">
+        <v>1</v>
+      </c>
+      <c r="F44">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="C46">
+        <v>4</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="C47">
+        <v>5</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="C48">
+        <v>6</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:6">
+      <c r="C49">
+        <v>7</v>
+      </c>
+      <c r="D49">
+        <v>2</v>
+      </c>
+      <c r="F49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:6">
+      <c r="C50" t="s">
+        <v>110</v>
+      </c>
+      <c r="D50">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
evaluaciones de impacto finales
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Usabilidad" sheetId="1" r:id="rId1"/>
@@ -2526,8 +2526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2576,8 +2576,14 @@
       <c r="D4">
         <v>1</v>
       </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
       <c r="F4">
         <v>5</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -2587,7 +2593,13 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
@@ -2598,7 +2610,13 @@
       <c r="D6">
         <v>2</v>
       </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>1</v>
       </c>
     </row>
@@ -2609,7 +2627,13 @@
       <c r="D7">
         <v>2</v>
       </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
       <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
     </row>
@@ -2620,7 +2644,13 @@
       <c r="D8">
         <v>2</v>
       </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
       <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
         <v>1</v>
       </c>
     </row>
@@ -2631,7 +2661,13 @@
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
       <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
         <v>1</v>
       </c>
     </row>
@@ -2642,7 +2678,13 @@
       <c r="D10">
         <v>2</v>
       </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
       <c r="F10">
+        <v>5</v>
+      </c>
+      <c r="G10">
         <v>5</v>
       </c>
     </row>
@@ -2653,6 +2695,9 @@
       <c r="D11">
         <v>13</v>
       </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
@@ -2664,6 +2709,15 @@
       <c r="D13">
         <v>2</v>
       </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:7">
       <c r="C14">
@@ -2672,8 +2726,14 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
       <c r="F14">
         <v>1</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -2683,8 +2743,14 @@
       <c r="D15">
         <v>2</v>
       </c>
+      <c r="E15">
+        <v>2</v>
+      </c>
       <c r="F15">
         <v>2</v>
+      </c>
+      <c r="G15">
+        <v>3</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -2694,52 +2760,79 @@
       <c r="D16">
         <v>1</v>
       </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
       <c r="F16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17">
+        <v>2</v>
+      </c>
       <c r="F17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="C18">
         <v>6</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
       <c r="F18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="C19">
         <v>7</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
       <c r="F19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="C20" t="s">
         <v>104</v>
       </c>
       <c r="D20">
         <v>11</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="E20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>106</v>
       </c>
@@ -2749,96 +2842,147 @@
       <c r="D22">
         <v>1</v>
       </c>
+      <c r="E22">
+        <v>2</v>
+      </c>
       <c r="F22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="G22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="C23">
         <v>2</v>
       </c>
       <c r="D23">
         <v>2</v>
       </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
       <c r="F23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="C24">
         <v>3</v>
       </c>
       <c r="D24">
         <v>2</v>
       </c>
+      <c r="E24">
+        <v>2</v>
+      </c>
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="C25">
         <v>4</v>
       </c>
       <c r="D25">
         <v>1</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
       </c>
       <c r="F25">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="C26">
         <v>5</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
       <c r="F26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="C27">
         <v>6</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
+      <c r="E27">
+        <v>2</v>
+      </c>
       <c r="F27">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="C28">
         <v>7</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <v>2</v>
+      </c>
       <c r="F28">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="C29">
         <v>8</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
       <c r="F29">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="C30" t="s">
         <v>110</v>
       </c>
       <c r="D30">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:6">
+      <c r="E30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>108</v>
       </c>
@@ -2848,96 +2992,147 @@
       <c r="D32">
         <v>1</v>
       </c>
+      <c r="E32">
+        <v>2</v>
+      </c>
       <c r="F32">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="G32">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="C33">
         <v>2</v>
       </c>
       <c r="D33">
         <v>1</v>
+      </c>
+      <c r="E33">
+        <v>2</v>
       </c>
       <c r="F33">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="C34">
         <v>3</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
+      <c r="E34">
+        <v>2</v>
+      </c>
       <c r="F34">
         <v>5</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="C35">
         <v>4</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
+      <c r="E35">
+        <v>2</v>
+      </c>
       <c r="F35">
         <v>2</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="C36">
         <v>5</v>
       </c>
       <c r="D36">
         <v>2</v>
       </c>
+      <c r="E36">
+        <v>2</v>
+      </c>
       <c r="F36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="C37">
         <v>6</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
       <c r="F37">
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="C38">
         <v>7</v>
       </c>
       <c r="D38">
         <v>1</v>
       </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
       <c r="F38">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="C39">
         <v>8</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
       <c r="F39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="C40" t="s">
         <v>110</v>
       </c>
       <c r="D40">
         <v>7</v>
       </c>
-    </row>
-    <row r="42" spans="1:6">
+      <c r="E40">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>109</v>
       </c>
@@ -2947,82 +3142,127 @@
       <c r="D42">
         <v>2</v>
       </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
       <c r="F42">
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="C43">
         <v>2</v>
       </c>
       <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
         <v>1</v>
       </c>
       <c r="F43">
         <v>3.5</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="C44">
         <v>3</v>
       </c>
       <c r="D44">
+        <v>2</v>
+      </c>
+      <c r="E44">
         <v>2</v>
       </c>
       <c r="F44">
         <v>8</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="C45">
         <v>4</v>
       </c>
       <c r="D45">
         <v>2</v>
       </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
       <c r="F45">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="C46">
         <v>5</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
       <c r="F46">
         <v>0</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="C47">
         <v>6</v>
       </c>
       <c r="D47">
         <v>1</v>
       </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
       <c r="F47">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="C48">
         <v>7</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="3:4">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:5">
       <c r="C49" t="s">
         <v>110</v>
       </c>
       <c r="D49">
         <v>10</v>
+      </c>
+      <c r="E49">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4072,7 +4312,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+    <sheetView topLeftCell="A35" workbookViewId="0">
       <selection activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
@@ -4585,8 +4825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="F50" sqref="F50"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4635,8 +4875,14 @@
       <c r="D4">
         <v>2</v>
       </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
       <c r="F4">
         <v>4</v>
+      </c>
+      <c r="G4">
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -4646,7 +4892,13 @@
       <c r="D5">
         <v>2</v>
       </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
       <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
         <v>1</v>
       </c>
     </row>
@@ -4657,7 +4909,13 @@
       <c r="D6">
         <v>2</v>
       </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
       <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
         <v>1</v>
       </c>
     </row>
@@ -4668,7 +4926,13 @@
       <c r="D7">
         <v>2</v>
       </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
       <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
         <v>4</v>
       </c>
     </row>
@@ -4679,8 +4943,14 @@
       <c r="D8">
         <v>2</v>
       </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
       <c r="F8">
         <v>4</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -4690,8 +4960,14 @@
       <c r="D9">
         <v>2</v>
       </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
       <c r="F9">
         <v>3</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -4701,8 +4977,14 @@
       <c r="D10">
         <v>1</v>
       </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
       <c r="F10">
         <v>4</v>
+      </c>
+      <c r="G10">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -4712,6 +4994,9 @@
       <c r="D11">
         <v>13</v>
       </c>
+      <c r="E11">
+        <v>14</v>
+      </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
@@ -4723,7 +5008,13 @@
       <c r="D13">
         <v>2</v>
       </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
       <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
         <v>1</v>
       </c>
     </row>
@@ -4734,8 +5025,14 @@
       <c r="D14">
         <v>1</v>
       </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
       <c r="F14">
         <v>2</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -4745,7 +5042,13 @@
       <c r="D15">
         <v>1</v>
       </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
       <c r="F15">
+        <v>2</v>
+      </c>
+      <c r="G15">
         <v>2</v>
       </c>
     </row>
@@ -4756,60 +5059,90 @@
       <c r="D16">
         <v>2</v>
       </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
       <c r="F16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="G16">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="C17">
         <v>5</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
       <c r="F17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="C18">
         <v>6</v>
       </c>
       <c r="D18">
         <v>2</v>
       </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
       <c r="F18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="C19">
         <v>7</v>
       </c>
       <c r="D19">
         <v>2</v>
       </c>
+      <c r="E19">
+        <v>2</v>
+      </c>
       <c r="F19">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="C20" t="s">
         <v>104</v>
       </c>
       <c r="D20">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="E20">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="C21" t="s">
         <v>110</v>
       </c>
       <c r="D21">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:6">
+      <c r="E21">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -4819,96 +5152,147 @@
       <c r="D23">
         <v>1</v>
       </c>
+      <c r="E23">
+        <v>2</v>
+      </c>
       <c r="F23">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="C24">
         <v>2</v>
       </c>
       <c r="D24">
         <v>1</v>
+      </c>
+      <c r="E24">
+        <v>2</v>
       </c>
       <c r="F24">
         <v>1.5</v>
       </c>
-    </row>
-    <row r="25" spans="1:6">
+      <c r="G24">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="C25">
         <v>3</v>
       </c>
       <c r="D25">
         <v>2</v>
       </c>
+      <c r="E25">
+        <v>2</v>
+      </c>
       <c r="F25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:6">
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="C26">
         <v>4</v>
       </c>
       <c r="D26">
         <v>2</v>
       </c>
+      <c r="E26">
+        <v>2</v>
+      </c>
       <c r="F26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:6">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="C27">
         <v>5</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
       <c r="F27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:6">
+      <c r="G27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="C28">
         <v>6</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
       <c r="F28">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="C29">
         <v>7</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
       <c r="F29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:6">
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="C30">
         <v>8</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
       <c r="F30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:6">
+      <c r="G30">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="C31" t="s">
         <v>110</v>
       </c>
       <c r="D31">
         <v>7</v>
       </c>
-    </row>
-    <row r="33" spans="1:6">
+      <c r="E31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>108</v>
       </c>
@@ -4918,96 +5302,147 @@
       <c r="D33">
         <v>1</v>
       </c>
+      <c r="E33">
+        <v>2</v>
+      </c>
       <c r="F33">
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:6">
+      <c r="G33">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="C34">
         <v>2</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
       <c r="F34">
         <v>4</v>
       </c>
-    </row>
-    <row r="35" spans="1:6">
+      <c r="G34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="C35">
         <v>3</v>
       </c>
       <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
         <v>1</v>
       </c>
       <c r="F35">
         <v>6</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="C36">
         <v>4</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
       <c r="F36">
         <v>4</v>
       </c>
-    </row>
-    <row r="37" spans="1:6">
+      <c r="G36">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="C37">
         <v>5</v>
       </c>
       <c r="D37">
         <v>2</v>
       </c>
+      <c r="E37">
+        <v>2</v>
+      </c>
       <c r="F37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:6">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="C38">
         <v>6</v>
       </c>
       <c r="D38">
         <v>2</v>
       </c>
+      <c r="E38">
+        <v>2</v>
+      </c>
       <c r="F38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="C39">
         <v>7</v>
       </c>
       <c r="D39">
         <v>2</v>
       </c>
+      <c r="E39">
+        <v>2</v>
+      </c>
       <c r="F39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="C40">
         <v>8</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
       <c r="F40">
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="C41" t="s">
         <v>110</v>
       </c>
       <c r="D41">
         <v>10</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="E41">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>109</v>
       </c>
@@ -5017,82 +5452,127 @@
       <c r="D43">
         <v>2</v>
       </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
       <c r="F43">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:6">
+      <c r="G43">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="C44">
         <v>2</v>
       </c>
       <c r="D44">
         <v>1</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
       </c>
       <c r="F44">
         <v>6</v>
       </c>
-    </row>
-    <row r="45" spans="1:6">
+      <c r="G44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="C45">
         <v>3</v>
       </c>
       <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
         <v>2</v>
       </c>
       <c r="F45">
         <v>8</v>
       </c>
-    </row>
-    <row r="46" spans="1:6">
+      <c r="G45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="C46">
         <v>4</v>
       </c>
       <c r="D46">
         <v>2</v>
       </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
       <c r="F46">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:6">
+      <c r="G46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="C47">
         <v>5</v>
       </c>
       <c r="D47">
         <v>2</v>
       </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
       <c r="F47">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="C48">
         <v>6</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
       <c r="F48">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="3:6">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7">
       <c r="C49">
         <v>7</v>
       </c>
       <c r="D49">
         <v>2</v>
       </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
       <c r="F49">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="3:6">
+      <c r="G49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7">
       <c r="C50" t="s">
         <v>110</v>
       </c>
       <c r="D50">
         <v>13</v>
+      </c>
+      <c r="E50">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
avances resultados y graficar
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Usabilidad" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
   <si>
     <t>Usabilidad</t>
   </si>
@@ -368,6 +368,150 @@
   </si>
   <si>
     <t>8º</t>
+  </si>
+  <si>
+    <t>Abierta-1</t>
+  </si>
+  <si>
+    <t>Abierta.2</t>
+  </si>
+  <si>
+    <t>IV.7</t>
+  </si>
+  <si>
+    <t>IV.6</t>
+  </si>
+  <si>
+    <t>IV.5</t>
+  </si>
+  <si>
+    <t>IV.4</t>
+  </si>
+  <si>
+    <t>IV.3</t>
+  </si>
+  <si>
+    <t>IV.2</t>
+  </si>
+  <si>
+    <t>XIV.1</t>
+  </si>
+  <si>
+    <t>XIV.3</t>
+  </si>
+  <si>
+    <t>XIV.2</t>
+  </si>
+  <si>
+    <t>XIII</t>
+  </si>
+  <si>
+    <t>XII.2</t>
+  </si>
+  <si>
+    <t>XII.1</t>
+  </si>
+  <si>
+    <t>XI.3</t>
+  </si>
+  <si>
+    <t>XI.2</t>
+  </si>
+  <si>
+    <t>XI.1</t>
+  </si>
+  <si>
+    <t>X.3</t>
+  </si>
+  <si>
+    <t>X.2</t>
+  </si>
+  <si>
+    <t>X.1</t>
+  </si>
+  <si>
+    <t>IX.3</t>
+  </si>
+  <si>
+    <t>IX.2</t>
+  </si>
+  <si>
+    <t>IX.1</t>
+  </si>
+  <si>
+    <t>VIII.3</t>
+  </si>
+  <si>
+    <t>VIII.2</t>
+  </si>
+  <si>
+    <t>VIII.1</t>
+  </si>
+  <si>
+    <t>VII.3</t>
+  </si>
+  <si>
+    <t>VII.2</t>
+  </si>
+  <si>
+    <t>VII.1</t>
+  </si>
+  <si>
+    <t>VI.3</t>
+  </si>
+  <si>
+    <t>VI.2</t>
+  </si>
+  <si>
+    <t>VI.1</t>
+  </si>
+  <si>
+    <t>V.3</t>
+  </si>
+  <si>
+    <t>V.2</t>
+  </si>
+  <si>
+    <t>V.1</t>
+  </si>
+  <si>
+    <t>IV.1</t>
+  </si>
+  <si>
+    <t>III.4</t>
+  </si>
+  <si>
+    <t>III.3</t>
+  </si>
+  <si>
+    <t>III.2</t>
+  </si>
+  <si>
+    <t>III.1</t>
+  </si>
+  <si>
+    <t>II.5</t>
+  </si>
+  <si>
+    <t>II.4</t>
+  </si>
+  <si>
+    <t>II.3</t>
+  </si>
+  <si>
+    <t>II.2</t>
+  </si>
+  <si>
+    <t>II.1</t>
+  </si>
+  <si>
+    <t>I.3</t>
+  </si>
+  <si>
+    <t>I.2</t>
+  </si>
+  <si>
+    <t>I.1</t>
   </si>
 </sst>
 </file>
@@ -707,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="X2" sqref="X2:X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -732,6 +876,7 @@
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="23" width="5.140625" customWidth="1"/>
     <col min="24" max="24" width="5.28515625" customWidth="1"/>
+    <col min="25" max="25" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -2027,9 +2172,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AZ4" sqref="AZ4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
@@ -2043,149 +2186,149 @@
       <c r="D1">
         <v>3</v>
       </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-      <c r="N1">
-        <v>13</v>
-      </c>
-      <c r="O1">
-        <v>14</v>
-      </c>
-      <c r="P1">
-        <v>15</v>
-      </c>
-      <c r="Q1">
-        <v>16</v>
-      </c>
-      <c r="R1">
-        <v>17</v>
-      </c>
-      <c r="S1">
-        <v>18</v>
-      </c>
-      <c r="T1">
-        <v>19</v>
-      </c>
-      <c r="U1">
-        <v>20</v>
-      </c>
-      <c r="V1">
-        <v>21</v>
-      </c>
-      <c r="W1">
-        <v>22</v>
-      </c>
-      <c r="X1">
-        <v>23</v>
-      </c>
-      <c r="Y1">
-        <v>24</v>
-      </c>
-      <c r="Z1">
-        <v>25</v>
-      </c>
-      <c r="AA1">
-        <v>26</v>
-      </c>
-      <c r="AB1">
-        <v>27</v>
-      </c>
-      <c r="AC1">
-        <v>28</v>
-      </c>
-      <c r="AD1">
-        <v>29</v>
-      </c>
-      <c r="AE1">
-        <v>30</v>
-      </c>
-      <c r="AF1">
-        <v>31</v>
-      </c>
-      <c r="AG1">
-        <v>32</v>
-      </c>
-      <c r="AH1">
-        <v>33</v>
-      </c>
-      <c r="AI1">
-        <v>34</v>
-      </c>
-      <c r="AJ1">
-        <v>35</v>
-      </c>
-      <c r="AK1">
-        <v>36</v>
-      </c>
-      <c r="AL1">
-        <v>37</v>
-      </c>
-      <c r="AM1">
-        <v>38</v>
-      </c>
-      <c r="AN1">
-        <v>39</v>
-      </c>
-      <c r="AO1">
-        <v>40</v>
-      </c>
-      <c r="AP1">
-        <v>41</v>
-      </c>
-      <c r="AQ1">
-        <v>42</v>
-      </c>
-      <c r="AR1">
-        <v>43</v>
-      </c>
-      <c r="AS1">
-        <v>44</v>
-      </c>
-      <c r="AT1">
-        <v>45</v>
-      </c>
-      <c r="AU1">
-        <v>46</v>
-      </c>
-      <c r="AV1">
-        <v>47</v>
-      </c>
-      <c r="AW1">
-        <v>48</v>
-      </c>
-      <c r="AX1">
-        <v>49</v>
-      </c>
-      <c r="AY1">
-        <v>50</v>
-      </c>
-      <c r="AZ1">
-        <v>51</v>
+      <c r="E1" t="s">
+        <v>162</v>
+      </c>
+      <c r="F1" t="s">
+        <v>161</v>
+      </c>
+      <c r="G1" t="s">
+        <v>160</v>
+      </c>
+      <c r="H1" t="s">
+        <v>159</v>
+      </c>
+      <c r="I1" t="s">
+        <v>158</v>
+      </c>
+      <c r="J1" t="s">
+        <v>157</v>
+      </c>
+      <c r="K1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" t="s">
+        <v>154</v>
+      </c>
+      <c r="N1" t="s">
+        <v>153</v>
+      </c>
+      <c r="O1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>150</v>
+      </c>
+      <c r="R1" t="s">
+        <v>122</v>
+      </c>
+      <c r="S1" t="s">
+        <v>121</v>
+      </c>
+      <c r="T1" t="s">
+        <v>120</v>
+      </c>
+      <c r="U1" t="s">
+        <v>119</v>
+      </c>
+      <c r="V1" t="s">
+        <v>118</v>
+      </c>
+      <c r="W1" t="s">
+        <v>117</v>
+      </c>
+      <c r="X1" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>148</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>115</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:52">

</xml_diff>

<commit_message>
resultados de evaluacion de impacto
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Usabilidad" sheetId="1" r:id="rId1"/>
@@ -85,9 +85,6 @@
     <t>Más pasillos de laberinto.</t>
   </si>
   <si>
-    <t>Aprender. Enseñar a los hijso con el videojuego.</t>
-  </si>
-  <si>
     <t>El creador del videojuego hizo un buen trabajo.</t>
   </si>
   <si>
@@ -220,9 +217,6 @@
     <t>Que era desafiante, ponía aprueba el intelecto</t>
   </si>
   <si>
-    <t>Poner más cosas, pone rinstrucciones más claras. Más sonidos</t>
-  </si>
-  <si>
     <t>Orientación y Diversión</t>
   </si>
   <si>
@@ -512,6 +506,12 @@
   </si>
   <si>
     <t>I.1</t>
+  </si>
+  <si>
+    <t>Poner más cosas, poner instrucciones más claras. Más sonidos</t>
+  </si>
+  <si>
+    <t>Aprender. Enseñar a los hijos con el videojuego.</t>
   </si>
 </sst>
 </file>
@@ -851,8 +851,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AC13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X13"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AC8" sqref="AC8:AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -876,7 +876,11 @@
     <col min="22" max="22" width="5" customWidth="1"/>
     <col min="23" max="23" width="5.140625" customWidth="1"/>
     <col min="24" max="24" width="5.28515625" customWidth="1"/>
-    <col min="25" max="25" width="26.85546875" customWidth="1"/>
+    <col min="25" max="25" width="26.140625" customWidth="1"/>
+    <col min="26" max="26" width="54.42578125" customWidth="1"/>
+    <col min="27" max="27" width="56.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.85546875" customWidth="1"/>
+    <col min="29" max="29" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29">
@@ -887,7 +891,7 @@
         <v>16</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1">
         <v>1</v>
@@ -970,7 +974,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>15</v>
@@ -1030,28 +1034,28 @@
         <v>10</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="AA2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AB2" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="AC2" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:29">
@@ -1059,7 +1063,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>15</v>
@@ -1128,19 +1132,19 @@
         <v>10</v>
       </c>
       <c r="Y3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>161</v>
+      </c>
+      <c r="AB3" t="s">
         <v>64</v>
       </c>
-      <c r="Z3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>66</v>
-      </c>
       <c r="AC3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:29">
@@ -1148,10 +1152,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" s="3">
         <v>42668</v>
@@ -1217,19 +1221,19 @@
         <v>5</v>
       </c>
       <c r="Y4" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z4" t="s">
         <v>60</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>61</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>62</v>
       </c>
-      <c r="AB4" t="s">
-        <v>63</v>
-      </c>
       <c r="AC4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:29">
@@ -1237,7 +1241,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>15</v>
@@ -1306,19 +1310,19 @@
         <v>9</v>
       </c>
       <c r="Y5" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z5" t="s">
         <v>56</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>57</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>58</v>
       </c>
-      <c r="AB5" t="s">
-        <v>59</v>
-      </c>
       <c r="AC5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:29">
@@ -1326,7 +1330,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>15</v>
@@ -1386,28 +1390,28 @@
         <v>9</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="Z6" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA6" s="2" t="s">
+      <c r="AB6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB6" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="AC6" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:29">
@@ -1415,10 +1419,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D7" s="3">
         <v>42669</v>
@@ -1484,19 +1488,19 @@
         <v>10</v>
       </c>
       <c r="Y7" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z7" t="s">
         <v>52</v>
       </c>
-      <c r="Z7" t="s">
+      <c r="AA7" t="s">
         <v>53</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>54</v>
       </c>
-      <c r="AB7" t="s">
-        <v>55</v>
-      </c>
       <c r="AC7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:29">
@@ -1564,28 +1568,28 @@
         <v>10</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="Y8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z8" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA8" s="2" t="s">
+      <c r="AB8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AB8" s="2" t="s">
+      <c r="AC8" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="AC8" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:29">
@@ -1593,7 +1597,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>15</v>
@@ -1662,19 +1666,19 @@
         <v>9</v>
       </c>
       <c r="Y9" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z9" t="s">
         <v>39</v>
       </c>
-      <c r="Z9" t="s">
+      <c r="AA9" t="s">
         <v>40</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>41</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>42</v>
-      </c>
-      <c r="AC9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:29">
@@ -1682,7 +1686,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>15</v>
@@ -1751,19 +1755,19 @@
         <v>10</v>
       </c>
       <c r="Y10" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z10" t="s">
         <v>34</v>
       </c>
-      <c r="Z10" t="s">
+      <c r="AA10" t="s">
         <v>35</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>36</v>
       </c>
-      <c r="AB10" t="s">
+      <c r="AC10" t="s">
         <v>37</v>
-      </c>
-      <c r="AC10" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:29">
@@ -1771,7 +1775,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -1840,19 +1844,19 @@
         <v>9</v>
       </c>
       <c r="Y11" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z11" t="s">
         <v>22</v>
       </c>
-      <c r="Z11" t="s">
+      <c r="AA11" t="s">
         <v>23</v>
       </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>24</v>
       </c>
-      <c r="AB11" t="s">
+      <c r="AC11" t="s">
         <v>25</v>
-      </c>
-      <c r="AC11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:29">
@@ -1938,10 +1942,10 @@
         <v>19</v>
       </c>
       <c r="AB12" t="s">
+        <v>162</v>
+      </c>
+      <c r="AC12" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="AC12" s="2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:29">
@@ -1949,7 +1953,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>15</v>
@@ -2009,28 +2013,28 @@
         <v>2</v>
       </c>
       <c r="V13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="X13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Y13" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="W13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="X13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="Y13" s="2" t="s">
+      <c r="Z13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="Z13" s="2" t="s">
+      <c r="AA13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AA13" s="2" t="s">
+      <c r="AB13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AB13" s="2" t="s">
+      <c r="AC13" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="AC13" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2071,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2079,7 +2083,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2087,7 +2091,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2095,7 +2099,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2103,7 +2107,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2111,7 +2115,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2119,7 +2123,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2127,7 +2131,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -2135,7 +2139,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -2143,7 +2147,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -2151,7 +2155,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -2159,7 +2163,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -2172,7 +2176,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AY2" sqref="AY2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
@@ -2187,153 +2193,153 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="I1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="J1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="L1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="N1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="P1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Q1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="R1" t="s">
+        <v>120</v>
+      </c>
+      <c r="S1" t="s">
+        <v>119</v>
+      </c>
+      <c r="T1" t="s">
+        <v>118</v>
+      </c>
+      <c r="U1" t="s">
+        <v>117</v>
+      </c>
+      <c r="V1" t="s">
+        <v>116</v>
+      </c>
+      <c r="W1" t="s">
+        <v>115</v>
+      </c>
+      <c r="X1" t="s">
+        <v>147</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>132</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>131</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>130</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>129</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>128</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>127</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>126</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>125</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>124</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>121</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>123</v>
+      </c>
+      <c r="AX1" t="s">
         <v>122</v>
       </c>
-      <c r="S1" t="s">
-        <v>121</v>
-      </c>
-      <c r="T1" t="s">
-        <v>120</v>
-      </c>
-      <c r="U1" t="s">
-        <v>119</v>
-      </c>
-      <c r="V1" t="s">
-        <v>118</v>
-      </c>
-      <c r="W1" t="s">
-        <v>117</v>
-      </c>
-      <c r="X1" t="s">
-        <v>149</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>148</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>147</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>145</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>144</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>143</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>141</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>140</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>139</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>138</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>137</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>136</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>135</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>134</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>133</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>132</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>131</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>130</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>129</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>128</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>127</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>126</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>125</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>124</v>
-      </c>
       <c r="AY1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AZ1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:52">
       <c r="A2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2483,15 +2489,15 @@
         <v>5</v>
       </c>
       <c r="AY2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="AZ2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:52">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2641,10 +2647,10 @@
         <v>5</v>
       </c>
       <c r="AY3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AZ3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2664,38 +2670,38 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B9" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
   </sheetData>
@@ -2708,7 +2714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
@@ -2722,35 +2728,35 @@
         <v>42689</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -2872,7 +2878,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>13</v>
@@ -2883,7 +2889,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3005,7 +3011,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -3016,7 +3022,7 @@
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -3155,7 +3161,7 @@
     </row>
     <row r="30" spans="1:7">
       <c r="C30" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D30">
         <v>9</v>
@@ -3166,7 +3172,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -3305,7 +3311,7 @@
     </row>
     <row r="40" spans="1:7">
       <c r="C40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40">
         <v>7</v>
@@ -3316,7 +3322,7 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -3438,7 +3444,7 @@
     </row>
     <row r="49" spans="3:5">
       <c r="C49" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D49">
         <v>10</v>
@@ -3470,35 +3476,35 @@
         <v>42691</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -3578,7 +3584,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>10</v>
@@ -3586,7 +3592,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -3666,7 +3672,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20">
         <v>10</v>
@@ -3674,7 +3680,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="C21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D21">
         <v>20</v>
@@ -3682,7 +3688,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -3773,7 +3779,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31">
         <v>4</v>
@@ -3781,7 +3787,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -3872,7 +3878,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="C41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D41">
         <v>6</v>
@@ -3880,7 +3886,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -3960,7 +3966,7 @@
     </row>
     <row r="50" spans="3:6">
       <c r="C50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50">
         <v>9</v>
@@ -3989,35 +3995,35 @@
         <v>42689</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4097,7 +4103,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>13</v>
@@ -4105,7 +4111,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4185,7 +4191,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -4193,7 +4199,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="C21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D21">
         <v>24</v>
@@ -4201,7 +4207,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -4292,7 +4298,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31">
         <v>10</v>
@@ -4300,7 +4306,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4391,7 +4397,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="C41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D41">
         <v>8</v>
@@ -4399,7 +4405,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -4479,7 +4485,7 @@
     </row>
     <row r="50" spans="3:6">
       <c r="C50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50">
         <v>10</v>
@@ -4505,38 +4511,38 @@
         <v>9</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -4616,7 +4622,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>12</v>
@@ -4624,7 +4630,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -4704,7 +4710,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -4712,7 +4718,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="C21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D21">
         <v>23</v>
@@ -4720,7 +4726,7 @@
     </row>
     <row r="23" spans="1:6">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -4808,7 +4814,7 @@
     </row>
     <row r="31" spans="1:6">
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31">
         <v>13</v>
@@ -4816,7 +4822,7 @@
     </row>
     <row r="33" spans="1:6">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -4907,7 +4913,7 @@
     </row>
     <row r="41" spans="1:6">
       <c r="C41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -4915,7 +4921,7 @@
     </row>
     <row r="43" spans="1:6">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -4992,7 +4998,7 @@
     </row>
     <row r="50" spans="3:4">
       <c r="C50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50">
         <v>13</v>
@@ -5021,35 +5027,35 @@
         <v>42691</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="D1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="C3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -5171,7 +5177,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="C11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D11">
         <v>13</v>
@@ -5182,7 +5188,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -5304,7 +5310,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="C20" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D20">
         <v>11</v>
@@ -5315,7 +5321,7 @@
     </row>
     <row r="21" spans="1:7">
       <c r="C21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D21">
         <v>24</v>
@@ -5326,7 +5332,7 @@
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -5465,7 +5471,7 @@
     </row>
     <row r="31" spans="1:7">
       <c r="C31" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D31">
         <v>7</v>
@@ -5476,7 +5482,7 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33">
         <v>1</v>
@@ -5615,7 +5621,7 @@
     </row>
     <row r="41" spans="1:7">
       <c r="C41" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D41">
         <v>10</v>
@@ -5626,7 +5632,7 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C43">
         <v>1</v>
@@ -5748,7 +5754,7 @@
     </row>
     <row r="50" spans="3:7">
       <c r="C50" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D50">
         <v>13</v>

</xml_diff>

<commit_message>
fin de anexos y datois heuristicos
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="4"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Usabilidad" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="164">
   <si>
     <t>Usabilidad</t>
   </si>
@@ -512,6 +512,9 @@
   </si>
   <si>
     <t>Aprender. Enseñar a los hijos con el videojuego.</t>
+  </si>
+  <si>
+    <t>A</t>
   </si>
 </sst>
 </file>
@@ -2174,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ3"/>
+  <dimension ref="A1:AZ4"/>
   <sheetViews>
-    <sheetView topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AY2" sqref="AY2"/>
+    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
+      <selection activeCell="AY4" sqref="AY4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2651,6 +2654,146 @@
       </c>
       <c r="AZ3" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:52">
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4.5</v>
+      </c>
+      <c r="H4">
+        <v>5</v>
+      </c>
+      <c r="I4">
+        <v>3.5</v>
+      </c>
+      <c r="J4">
+        <v>5</v>
+      </c>
+      <c r="K4">
+        <v>3</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+      <c r="N4">
+        <v>5</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>3.5</v>
+      </c>
+      <c r="R4">
+        <v>3</v>
+      </c>
+      <c r="S4">
+        <v>4</v>
+      </c>
+      <c r="T4">
+        <v>4</v>
+      </c>
+      <c r="U4">
+        <v>4</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <v>4.5</v>
+      </c>
+      <c r="X4">
+        <v>5</v>
+      </c>
+      <c r="Y4">
+        <v>4.5</v>
+      </c>
+      <c r="Z4">
+        <v>5</v>
+      </c>
+      <c r="AA4">
+        <v>3.5</v>
+      </c>
+      <c r="AB4">
+        <v>5</v>
+      </c>
+      <c r="AC4">
+        <v>5</v>
+      </c>
+      <c r="AD4">
+        <v>5</v>
+      </c>
+      <c r="AE4">
+        <v>5</v>
+      </c>
+      <c r="AF4">
+        <v>5</v>
+      </c>
+      <c r="AG4">
+        <v>4.5</v>
+      </c>
+      <c r="AH4">
+        <v>5</v>
+      </c>
+      <c r="AI4">
+        <v>5</v>
+      </c>
+      <c r="AJ4">
+        <v>4.5</v>
+      </c>
+      <c r="AK4">
+        <v>5</v>
+      </c>
+      <c r="AL4">
+        <v>5</v>
+      </c>
+      <c r="AM4">
+        <v>5</v>
+      </c>
+      <c r="AN4">
+        <v>5</v>
+      </c>
+      <c r="AO4">
+        <v>5</v>
+      </c>
+      <c r="AP4">
+        <v>5</v>
+      </c>
+      <c r="AQ4">
+        <v>5</v>
+      </c>
+      <c r="AR4">
+        <v>5</v>
+      </c>
+      <c r="AS4">
+        <v>3</v>
+      </c>
+      <c r="AT4">
+        <v>3.5</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>163</v>
+      </c>
+      <c r="AV4">
+        <v>0</v>
+      </c>
+      <c r="AW4">
+        <v>5</v>
+      </c>
+      <c r="AX4">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2714,8 +2857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3462,8 +3605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="F54" sqref="F54"/>
+    <sheetView topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3981,8 +4124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -4500,8 +4643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="F45" sqref="F45"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5013,8 +5156,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43:E50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
se han anotado todos los resultados en el documento
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="164">
   <si>
     <t>Usabilidad</t>
   </si>
@@ -2177,10 +2177,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AZ4"/>
+  <dimension ref="A1:AZ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AG1" workbookViewId="0">
-      <selection activeCell="AY4" sqref="AY4"/>
+    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AV5" sqref="AV5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2793,6 +2793,50 @@
         <v>5</v>
       </c>
       <c r="AX4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:52">
+      <c r="G5">
+        <v>4.5</v>
+      </c>
+      <c r="L5">
+        <v>3.5</v>
+      </c>
+      <c r="P5">
+        <v>4.75</v>
+      </c>
+      <c r="W5">
+        <v>3.86</v>
+      </c>
+      <c r="Z5">
+        <v>4.83</v>
+      </c>
+      <c r="AC5">
+        <v>4.5</v>
+      </c>
+      <c r="AF5">
+        <v>5</v>
+      </c>
+      <c r="AI5">
+        <v>4.83</v>
+      </c>
+      <c r="AL5">
+        <v>4.83</v>
+      </c>
+      <c r="AO5">
+        <v>5</v>
+      </c>
+      <c r="AR5">
+        <v>5</v>
+      </c>
+      <c r="AT5">
+        <v>3.25</v>
+      </c>
+      <c r="AU5" t="s">
+        <v>163</v>
+      </c>
+      <c r="AX5">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
se termina evaluacion de resultados
</commit_message>
<xml_diff>
--- a/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
+++ b/Trabajo Memoria/Segundo Semestre/Evaluaciones.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="2"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Usabilidad" sheetId="1" r:id="rId1"/>
@@ -2179,8 +2179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AZ5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH1" workbookViewId="0">
-      <selection activeCell="AV5" sqref="AV5"/>
+    <sheetView topLeftCell="AH1" workbookViewId="0">
+      <selection activeCell="AL5" sqref="AL5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2901,8 +2901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E49"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -5200,7 +5200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G50"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
       <selection activeCell="D43" sqref="D43:E50"/>
     </sheetView>
   </sheetViews>

</xml_diff>